<commit_message>
deleted elements in materials for risks
</commit_message>
<xml_diff>
--- a/materials/specs/Green_Taxo.xlsx
+++ b/materials/specs/Green_Taxo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlorans\Documents\ClimateInvestingNLP\materials\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A025B537-684F-46AD-9A10-B92EB7AF4572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D839A75D-6826-4840-BBAA-242CE5596367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5750" yWindow="100" windowWidth="16920" windowHeight="10450" xr2:uid="{4FC0EE15-120B-4526-9ADE-E0ED7501A6A5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{4FC0EE15-120B-4526-9ADE-E0ED7501A6A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="132">
   <si>
     <t>Type</t>
   </si>
@@ -423,6 +423,15 @@
   </si>
   <si>
     <t>Professional services related to energy performance of buildings</t>
+  </si>
+  <si>
+    <t>Electric vehicles</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>companies engaged in exploration &amp; production, refining &amp; marketing, and storage &amp; transportation of oil &amp; gas and coal &amp; consumable fuels. It also includes companies that offer oil &amp; gas equipment and services.</t>
   </si>
 </sst>
 </file>
@@ -438,12 +447,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -458,8 +473,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -774,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A58CB6E-3A5C-483C-88CA-FB864E6C9536}">
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:XFD74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1574,6 +1590,25 @@
         <v>128</v>
       </c>
     </row>
+    <row r="73" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modified green taxo part
</commit_message>
<xml_diff>
--- a/materials/specs/Green_Taxo.xlsx
+++ b/materials/specs/Green_Taxo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlorans\Documents\ClimateInvestingNLP\materials\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883EB36A-1FCF-4A76-A2B4-22A5F518FEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2A1F38-5566-44C2-BAB6-E909995EE836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{4FC0EE15-120B-4526-9ADE-E0ED7501A6A5}"/>
   </bookViews>
@@ -837,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A58CB6E-3A5C-483C-88CA-FB864E6C9536}">
   <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>